<commit_message>
first (bad) speedup values
</commit_message>
<xml_diff>
--- a/APGAS/Speedup.xlsx
+++ b/APGAS/Speedup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\EinfParallel\EinfParaAPGAS_CUDA\APGAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB73EB3-2140-44E2-A5A7-BC449972E6C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12900A1-1F89-42B9-B72E-38B35954E7E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A24DB2A-7B28-45B5-9F05-5D37EA4C5777}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>1 Place</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>verbose</t>
+  </si>
+  <si>
+    <t>Speedup</t>
   </si>
 </sst>
 </file>
@@ -104,11 +107,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -423,15 +427,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9BFDFD-4745-4081-B6F7-E79D801FFF0C}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -442,8 +446,24 @@
       <c r="G1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1</v>
       </c>
@@ -459,95 +479,293 @@
       <c r="F2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="G4" t="e">
+      <c r="B4">
+        <v>0.22180293300000001</v>
+      </c>
+      <c r="G4">
         <f>SUM(B4:F4)/COUNTA(B4:F4)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.22180293300000001</v>
+      </c>
+      <c r="H4">
+        <f>G$4/G4</f>
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>23.713405121000001</v>
+      </c>
+      <c r="P4">
+        <f>SUM(K4:O4)/COUNTA(K4:O4)</f>
+        <v>23.713405121000001</v>
+      </c>
+      <c r="Q4">
+        <f>P$4/P4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="G5" t="e">
+      <c r="B5">
+        <v>0.20481740700000001</v>
+      </c>
+      <c r="G5">
         <f t="shared" ref="G5:G13" si="0">SUM(B5:F5)/COUNTA(B5:F5)</f>
+        <v>0.20481740700000001</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H13" si="1">G$4/G5</f>
+        <v>1.0829300900191554</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="P5" t="e">
+        <f t="shared" ref="P5:P13" si="2">SUM(K5:O5)/COUNTA(K5:O5)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="Q5" t="e">
+        <f t="shared" ref="Q5:Q13" si="3">P$4/P5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="G6" t="e">
+      <c r="B6">
+        <v>0.19969244799999999</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.19969244799999999</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>1.1107226899236571</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2">
+        <v>223.026686391</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="2"/>
+        <v>223.026686391</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="3"/>
+        <v>0.10632541560262776</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>8</v>
       </c>
-      <c r="G7" t="e">
+      <c r="B7">
+        <v>0.167936961</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.167936961</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1.320751141852567</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="K7" s="2">
+        <v>379.69189024799999</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>379.69189024799999</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="3"/>
+        <v>6.245433660832557E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>16</v>
       </c>
-      <c r="G8" t="e">
+      <c r="B8">
+        <v>0.20255146199999999</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.20255146199999999</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1.0950448385309608</v>
+      </c>
+      <c r="J8">
+        <v>16</v>
+      </c>
+      <c r="K8" s="2">
+        <v>389.67092231300001</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>389.67092231300001</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="3"/>
+        <v>6.0854951609533754E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>32</v>
       </c>
-      <c r="G9" t="e">
+      <c r="B9">
+        <v>0.21104368200000001</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.21104368200000001</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1.050981156592975</v>
+      </c>
+      <c r="J9">
+        <v>32</v>
+      </c>
+      <c r="K9" s="2">
+        <v>397.11087480800001</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="2"/>
+        <v>397.11087480800001</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="3"/>
+        <v>5.9714821792440829E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>32</v>
       </c>
-      <c r="G11" t="e">
+      <c r="B11">
+        <v>0.62595568400000001</v>
+      </c>
+      <c r="C11">
+        <v>0.59221459099999996</v>
+      </c>
+      <c r="D11">
+        <v>0.58888607599999998</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.60235211700000002</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0.36822802932059756</v>
+      </c>
+      <c r="J11">
+        <v>32</v>
+      </c>
+      <c r="K11" s="2">
+        <v>199.253641429</v>
+      </c>
+      <c r="P11">
+        <f t="shared" ref="P11:P16" si="4">SUM(K11:O11)/COUNTA(K11:O11)</f>
+        <v>199.253641429</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="3"/>
+        <v>0.11901115056634884</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>32</v>
       </c>
-      <c r="G13" t="e">
+      <c r="B13">
+        <v>0.56563673400000003</v>
+      </c>
+      <c r="C13">
+        <v>0.60348345800000003</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.58456009600000003</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0.379435638042594</v>
+      </c>
+      <c r="J13">
+        <v>32</v>
+      </c>
+      <c r="K13" s="2">
+        <v>103.400613564</v>
+      </c>
+      <c r="P13">
+        <f t="shared" ref="P13:P16" si="5">SUM(K13:O13)/COUNTA(K13:O13)</f>
+        <v>103.400613564</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="3"/>
+        <v>0.22933524573645345</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -569,10 +787,70 @@
       <c r="G15" t="s">
         <v>11</v>
       </c>
+      <c r="J15" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N15" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" t="s">
+        <v>10</v>
+      </c>
+      <c r="P15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+      <c r="L16">
+        <v>10</v>
+      </c>
+      <c r="M16">
+        <v>42</v>
+      </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
+      <c r="O16">
+        <v>10</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
+    <mergeCell ref="K1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>